<commit_message>
multiple updates made to application_data_condensed_df
</commit_message>
<xml_diff>
--- a/application_data_condensed_student_applicants_df.xlsx
+++ b/application_data_condensed_student_applicants_df.xlsx
@@ -202,22 +202,22 @@
     <t>14:00:00</t>
   </si>
   <si>
-    <t>9:00:00</t>
+    <t>09:00:00</t>
   </si>
   <si>
     <t>11:00:00</t>
   </si>
   <si>
-    <t>6:00:00</t>
-  </si>
-  <si>
-    <t>7:00:00</t>
+    <t>06:00:00</t>
+  </si>
+  <si>
+    <t>07:00:00</t>
   </si>
   <si>
     <t>12:00:00</t>
   </si>
   <si>
-    <t>8:00:00</t>
+    <t>08:00:00</t>
   </si>
   <si>
     <t>Business Entity Type 2</t>

</xml_diff>